<commit_message>
correcao e adicao de funcao para conexao com o banco
</commit_message>
<xml_diff>
--- a/excel/planilhasGerada/importar-parceiros-teste.xlsx
+++ b/excel/planilhasGerada/importar-parceiros-teste.xlsx
@@ -900,51 +900,129 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Fornecedor</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>619.574.283-09</t>
+          <t>32.159.486/0001-00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Isabel Moura</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>Lorenzo Almeida</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>enhance holistic e-tailers</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>4530706</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>9363</v>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" s="6" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" s="6" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" s="6" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" s="6" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+          <t>Não Contribuinte</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>7167</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>87866990</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Sr. Yago Almeida</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>64.390.152/0001-20</t>
+        </is>
+      </c>
+      <c r="O3" s="6" t="inlineStr">
+        <is>
+          <t>re-intermediate bleeding-edge models</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>2112893390</v>
+      </c>
+      <c r="S3" s="6" t="inlineStr">
+        <is>
+          <t>mendesbryan@bol.com.br</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>COMERCIAL</t>
+        </is>
+      </c>
+      <c r="U3" s="6" t="inlineStr">
+        <is>
+          <t>41072536</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Vereda de Fernandes</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>RSZVI5QZP1</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Santa Margarida</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Lagoinha Leblon</t>
+        </is>
+      </c>
+      <c r="AA3" s="6" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" t="inlineStr">
@@ -954,53 +1032,121 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fornecedor</t>
+          <t>Cliente | Transportadora</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Pessoa Física</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>269.810.543-70</t>
+          <t>38192074579</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Leandro Moura</t>
+          <t>Sophia Silva</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>3706</v>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>Contribuinte</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>5873</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" s="6" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" s="6" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" s="6" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" s="6" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
+        <v>2135</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>87866990</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>João Felipe Rocha</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>09134852689</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
+          <t>visualize customized experiences</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>13513451737</v>
+      </c>
+      <c r="S4" s="6" t="inlineStr">
+        <is>
+          <t>enrico61@yahoo.com.br</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>ENTREGA</t>
+        </is>
+      </c>
+      <c r="U4" s="6" t="inlineStr">
+        <is>
+          <t>84947550</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Pátio Nascimento</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>FSNMY75JIN</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Vila São Francisco</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Atila De Paiva</t>
+        </is>
+      </c>
+      <c r="AA4" s="6" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" t="inlineStr">
@@ -1010,53 +1156,119 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fornecedor | Transportadora</t>
+          <t>Cliente | Fornecedor | Transportadora</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Estrangeiro</t>
+          <t>Pessoa Jurídica</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>64250987329</t>
+          <t>37.216.084/0001-05</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Francisco Azevedo</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>Joana Almeida</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>incubate wireless interfaces</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>4530706</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>6877</v>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>Contribuinte</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>3744</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" s="6" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+        <v>7130</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>82252918</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Ana Lívia Lopes</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>92.501.836/0001-98</t>
+        </is>
+      </c>
+      <c r="O5" s="6" t="inlineStr">
+        <is>
+          <t>incubate clicks-and-mortar supply-chains</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
       <c r="S5" s="6" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" s="6" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" s="6" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>RESIDENCIAL</t>
+        </is>
+      </c>
+      <c r="U5" s="6" t="inlineStr">
+        <is>
+          <t>24062868</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Aeroporto da Costa</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>LM3A5A48JB</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Vila Batik</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Marçola</t>
+        </is>
+      </c>
+      <c r="AA5" s="6" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" t="inlineStr">
@@ -1066,28 +1278,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Transportadora</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Pessoa Jurídica</t>
+          <t>Estrangeiro</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27.601.938/0001-13</t>
+          <t>78523109668</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mariane da Rosa</t>
+          <t>Dra. Alícia da Cunha</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>855</v>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>Isento</t>
@@ -1095,22 +1309,84 @@
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" s="6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" s="6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" s="6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Caio Cavalcanti</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>15809276377</t>
+        </is>
+      </c>
+      <c r="O6" s="6" t="inlineStr">
+        <is>
+          <t>re-contextualize real-time channels</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Celular</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
+        <v>11594431510</v>
+      </c>
+      <c r="S6" s="6" t="inlineStr">
+        <is>
+          <t>rochadiogo@yahoo.com.br</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>OUTROS</t>
+        </is>
+      </c>
+      <c r="U6" s="6" t="inlineStr">
+        <is>
+          <t>12342738</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Núcleo de da Rocha</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>O4ARVFVVYJ</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Vila Jardim São José</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Dom Joaquim</t>
+        </is>
+      </c>
+      <c r="AA6" s="6" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" t="inlineStr">
@@ -1120,7 +1396,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cliente | Fornecedor</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1130,18 +1406,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>238.705.916-68</t>
+          <t>649.381.057-48</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Caroline Moura</t>
+          <t>Fernanda Moraes</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>09/03/1995</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>349</v>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
           <t>Isento</t>
@@ -1149,576 +1431,144 @@
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" s="6" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" s="6" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" s="6" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" s="6" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Luiz Felipe Nogueira</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>497.315.068-10</t>
+        </is>
+      </c>
+      <c r="O7" s="6" t="inlineStr">
+        <is>
+          <t>mesh user-centric experiences</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Celular</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>1774457052</v>
+      </c>
+      <c r="S7" s="6" t="inlineStr">
+        <is>
+          <t>poliveira@ig.com.br</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>ENTREGA</t>
+        </is>
+      </c>
+      <c r="U7" s="6" t="inlineStr">
+        <is>
+          <t>12150628</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Aeroporto Correia</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>6K749VQARX</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Tirol</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Marieta 3ª Seção</t>
+        </is>
+      </c>
+      <c r="AA7" s="6" t="inlineStr">
+        <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Cliente | Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>476.153.892-91</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Lucas Gabriel Barbosa</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>2620</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" s="6" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" s="6" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" s="6" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" s="6" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
+      <c r="O8" s="6" t="n"/>
+      <c r="S8" s="6" t="n"/>
+      <c r="U8" s="6" t="n"/>
+      <c r="AA8" s="6" t="n"/>
     </row>
     <row r="9" ht="30" customHeight="1">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Cliente | Fornecedor</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>61.038.927/0001-05</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Maitê Jesus</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>3222</v>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" s="6" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" s="6" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" s="6" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" s="6" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
+      <c r="O9" s="6" t="n"/>
+      <c r="S9" s="6" t="n"/>
+      <c r="U9" s="6" t="n"/>
+      <c r="AA9" s="6" t="n"/>
     </row>
     <row r="10" ht="30" customHeight="1">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cliente | Transportadora</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>01843957205</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Dra. Isadora da Mata</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>5116</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" s="6" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" s="6" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" s="6" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" s="6" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
+      <c r="O10" s="6" t="n"/>
+      <c r="S10" s="6" t="n"/>
+      <c r="U10" s="6" t="n"/>
+      <c r="AA10" s="6" t="n"/>
     </row>
     <row r="11" ht="30" customHeight="1">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>518.294.670-85</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Igor Rocha</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Não Contribuinte</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>1967</v>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" s="6" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" s="6" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" s="6" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" s="6" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
+      <c r="O11" s="6" t="n"/>
+      <c r="S11" s="6" t="n"/>
+      <c r="U11" s="6" t="n"/>
+      <c r="AA11" s="6" t="n"/>
     </row>
     <row r="12" ht="30" customHeight="1">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>83546970292</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Gabriel Gonçalves</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>1789</v>
-      </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" s="6" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" s="6" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" s="6" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" s="6" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
+      <c r="O12" s="6" t="n"/>
+      <c r="S12" s="6" t="n"/>
+      <c r="U12" s="6" t="n"/>
+      <c r="AA12" s="6" t="n"/>
     </row>
     <row r="13" ht="30" customHeight="1">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Cliente | Transportadora</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>079.856.243-92</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Isabella Lima</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" s="6" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" s="6" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" s="6" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" s="6" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
+      <c r="O13" s="6" t="n"/>
+      <c r="S13" s="6" t="n"/>
+      <c r="U13" s="6" t="n"/>
+      <c r="AA13" s="6" t="n"/>
     </row>
     <row r="14" ht="30" customHeight="1">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Cliente | Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Pessoa Jurídica</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>57.280.416/0001-28</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Vinicius Teixeira</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>7928</v>
-      </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" s="6" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" s="6" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" s="6" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" s="6" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
+      <c r="O14" s="6" t="n"/>
+      <c r="S14" s="6" t="n"/>
+      <c r="U14" s="6" t="n"/>
+      <c r="AA14" s="6" t="n"/>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Cliente | Fornecedor</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>543.782.096-83</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Sra. Esther da Rocha</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Contribuinte</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>6570</v>
-      </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" s="6" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" s="6" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" s="6" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" s="6" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
+      <c r="O15" s="6" t="n"/>
+      <c r="S15" s="6" t="n"/>
+      <c r="U15" s="6" t="n"/>
+      <c r="AA15" s="6" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Transportadora</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Pessoa Física</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>409.318.627-87</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Antônio Araújo</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" s="6" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" s="6" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" s="6" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" s="6" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
+      <c r="O16" s="6" t="n"/>
+      <c r="S16" s="6" t="n"/>
+      <c r="U16" s="6" t="n"/>
+      <c r="AA16" s="6" t="n"/>
     </row>
     <row r="17" ht="30" customHeight="1">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Fornecedor | Transportadora</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Estrangeiro</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>48952671058</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Ana Sophia Souza</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Isento</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" s="6" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" s="6" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" s="6" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" s="6" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
+      <c r="O17" s="6" t="n"/>
+      <c r="S17" s="6" t="n"/>
+      <c r="U17" s="6" t="n"/>
+      <c r="AA17" s="6" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="O18" s="6" t="n"/>

</xml_diff>